<commit_message>
Accidental update, no change
</commit_message>
<xml_diff>
--- a/Lab03/7seg_Values.xlsx
+++ b/Lab03/7seg_Values.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/g_tec/Git/PLK_lab/Lab03/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4493143B-8305-D44C-BFB1-16F7E60CA38B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F800AE98-5C92-8549-B4B3-0D3140084C35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4420" yWindow="1040" windowWidth="32280" windowHeight="23840" xr2:uid="{92F74FB5-F906-4D4D-B742-F0F267F06BF9}"/>
+    <workbookView xWindow="20120" yWindow="880" windowWidth="32280" windowHeight="23840" xr2:uid="{92F74FB5-F906-4D4D-B742-F0F267F06BF9}"/>
   </bookViews>
   <sheets>
     <sheet name="Part5" sheetId="1" r:id="rId1"/>
@@ -253,6 +253,19 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -260,19 +273,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -612,7 +612,7 @@
   <dimension ref="B1:X24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="112" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -672,36 +672,36 @@
       <c r="D6" s="4"/>
     </row>
     <row r="7" spans="2:24" ht="22">
-      <c r="F7" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="G7" s="7" t="s">
+      <c r="F7" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="G7" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="H7" s="7"/>
-      <c r="I7" s="7"/>
-      <c r="J7" s="7"/>
-      <c r="K7" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="L7" s="7"/>
-      <c r="M7" s="7"/>
-      <c r="N7" s="7"/>
-      <c r="O7" s="7"/>
-      <c r="P7" s="7"/>
-      <c r="Q7" s="8"/>
+      <c r="H7" s="12"/>
+      <c r="I7" s="12"/>
+      <c r="J7" s="12"/>
+      <c r="K7" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="L7" s="12"/>
+      <c r="M7" s="12"/>
+      <c r="N7" s="12"/>
+      <c r="O7" s="12"/>
+      <c r="P7" s="12"/>
+      <c r="Q7" s="13"/>
       <c r="R7" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="S7" s="9"/>
-      <c r="T7" s="9"/>
-      <c r="U7" s="9"/>
-      <c r="V7" s="9"/>
-      <c r="W7" s="9"/>
-      <c r="X7" s="9"/>
+      <c r="S7" s="7"/>
+      <c r="T7" s="7"/>
+      <c r="U7" s="7"/>
+      <c r="V7" s="7"/>
+      <c r="W7" s="7"/>
+      <c r="X7" s="7"/>
     </row>
     <row r="8" spans="2:24" ht="22" customHeight="1">
-      <c r="F8" s="6"/>
+      <c r="F8" s="11"/>
       <c r="G8" s="2">
         <v>3</v>
       </c>
@@ -732,7 +732,7 @@
       <c r="P8" s="2">
         <v>1</v>
       </c>
-      <c r="Q8" s="10">
+      <c r="Q8" s="6">
         <v>0</v>
       </c>
       <c r="R8" s="2" t="s">
@@ -773,10 +773,10 @@
       <c r="P9" s="3">
         <v>0</v>
       </c>
-      <c r="Q9" s="11">
-        <v>0</v>
-      </c>
-      <c r="R9" s="13" t="s">
+      <c r="Q9" s="8">
+        <v>0</v>
+      </c>
+      <c r="R9" s="10" t="s">
         <v>11</v>
       </c>
     </row>
@@ -814,10 +814,10 @@
       <c r="P10" s="3">
         <v>0</v>
       </c>
-      <c r="Q10" s="11">
-        <v>1</v>
-      </c>
-      <c r="R10" s="13" t="s">
+      <c r="Q10" s="8">
+        <v>1</v>
+      </c>
+      <c r="R10" s="10" t="s">
         <v>12</v>
       </c>
     </row>
@@ -855,10 +855,10 @@
       <c r="P11" s="3">
         <v>0</v>
       </c>
-      <c r="Q11" s="11">
-        <v>0</v>
-      </c>
-      <c r="R11" s="13" t="s">
+      <c r="Q11" s="8">
+        <v>0</v>
+      </c>
+      <c r="R11" s="10" t="s">
         <v>13</v>
       </c>
     </row>
@@ -896,10 +896,10 @@
       <c r="P12" s="3">
         <v>0</v>
       </c>
-      <c r="Q12" s="11">
-        <v>0</v>
-      </c>
-      <c r="R12" s="13" t="s">
+      <c r="Q12" s="8">
+        <v>0</v>
+      </c>
+      <c r="R12" s="10" t="s">
         <v>14</v>
       </c>
     </row>
@@ -937,10 +937,10 @@
       <c r="P13" s="3">
         <v>0</v>
       </c>
-      <c r="Q13" s="11">
-        <v>1</v>
-      </c>
-      <c r="R13" s="13" t="s">
+      <c r="Q13" s="8">
+        <v>1</v>
+      </c>
+      <c r="R13" s="10" t="s">
         <v>15</v>
       </c>
     </row>
@@ -978,10 +978,10 @@
       <c r="P14" s="3">
         <v>1</v>
       </c>
-      <c r="Q14" s="11">
-        <v>0</v>
-      </c>
-      <c r="R14" s="13" t="s">
+      <c r="Q14" s="8">
+        <v>0</v>
+      </c>
+      <c r="R14" s="10" t="s">
         <v>16</v>
       </c>
     </row>
@@ -1019,10 +1019,10 @@
       <c r="P15" s="3">
         <v>1</v>
       </c>
-      <c r="Q15" s="12">
-        <v>1</v>
-      </c>
-      <c r="R15" s="13" t="s">
+      <c r="Q15" s="9">
+        <v>1</v>
+      </c>
+      <c r="R15" s="10" t="s">
         <v>17</v>
       </c>
     </row>
@@ -1060,10 +1060,10 @@
       <c r="P16" s="3">
         <v>0</v>
       </c>
-      <c r="Q16" s="11">
-        <v>0</v>
-      </c>
-      <c r="R16" s="13" t="s">
+      <c r="Q16" s="8">
+        <v>0</v>
+      </c>
+      <c r="R16" s="10" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1101,10 +1101,10 @@
       <c r="P17" s="3">
         <v>0</v>
       </c>
-      <c r="Q17" s="11">
-        <v>0</v>
-      </c>
-      <c r="R17" s="13" t="s">
+      <c r="Q17" s="8">
+        <v>0</v>
+      </c>
+      <c r="R17" s="10" t="s">
         <v>19</v>
       </c>
     </row>
@@ -1142,10 +1142,10 @@
       <c r="P18" s="3">
         <v>0</v>
       </c>
-      <c r="Q18" s="11">
-        <v>0</v>
-      </c>
-      <c r="R18" s="13" t="s">
+      <c r="Q18" s="8">
+        <v>0</v>
+      </c>
+      <c r="R18" s="10" t="s">
         <v>20</v>
       </c>
     </row>
@@ -1183,10 +1183,10 @@
       <c r="P19" s="3">
         <v>0</v>
       </c>
-      <c r="Q19" s="11">
-        <v>0</v>
-      </c>
-      <c r="R19" s="13" t="s">
+      <c r="Q19" s="8">
+        <v>0</v>
+      </c>
+      <c r="R19" s="10" t="s">
         <v>21</v>
       </c>
     </row>
@@ -1224,10 +1224,10 @@
       <c r="P20" s="3">
         <v>1</v>
       </c>
-      <c r="Q20" s="11">
-        <v>1</v>
-      </c>
-      <c r="R20" s="13" t="s">
+      <c r="Q20" s="8">
+        <v>1</v>
+      </c>
+      <c r="R20" s="10" t="s">
         <v>17</v>
       </c>
     </row>
@@ -1265,10 +1265,10 @@
       <c r="P21" s="3">
         <v>1</v>
       </c>
-      <c r="Q21" s="11">
-        <v>0</v>
-      </c>
-      <c r="R21" s="13" t="s">
+      <c r="Q21" s="8">
+        <v>0</v>
+      </c>
+      <c r="R21" s="10" t="s">
         <v>22</v>
       </c>
     </row>
@@ -1306,10 +1306,10 @@
       <c r="P22" s="3">
         <v>0</v>
       </c>
-      <c r="Q22" s="11">
-        <v>1</v>
-      </c>
-      <c r="R22" s="13" t="s">
+      <c r="Q22" s="8">
+        <v>1</v>
+      </c>
+      <c r="R22" s="10" t="s">
         <v>23</v>
       </c>
     </row>
@@ -1347,10 +1347,10 @@
       <c r="P23" s="3">
         <v>1</v>
       </c>
-      <c r="Q23" s="11">
-        <v>0</v>
-      </c>
-      <c r="R23" s="13" t="s">
+      <c r="Q23" s="8">
+        <v>0</v>
+      </c>
+      <c r="R23" s="10" t="s">
         <v>24</v>
       </c>
     </row>
@@ -1388,10 +1388,10 @@
       <c r="P24" s="3">
         <v>1</v>
       </c>
-      <c r="Q24" s="11">
-        <v>0</v>
-      </c>
-      <c r="R24" s="13" t="s">
+      <c r="Q24" s="8">
+        <v>0</v>
+      </c>
+      <c r="R24" s="10" t="s">
         <v>25</v>
       </c>
     </row>

</xml_diff>